<commit_message>
Added homology model classification
</commit_message>
<xml_diff>
--- a/data/redone_excel_sheets/hm/set_comparison_7feats_v2.1.1_Set2_hm_10belly_capped.xlsx
+++ b/data/redone_excel_sheets/hm/set_comparison_7feats_v2.1.1_Set2_hm_10belly_capped.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livememphis-my.sharepoint.com/personal/gszwbwsk_memphis_edu/Documents/SBP/score_based_ph4/score_sheets/latest_script_data/7feats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livememphis-my.sharepoint.com/personal/gszwbwsk_memphis_edu/Documents/Machine Learning/ph4_classification/data/redone_excel_sheets/hm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="8_{C4217763-33D1-4FEB-9876-BB3C3C40EE23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B56C2EC3-3003-4E2F-BCA9-821799D641E7}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{C4217763-33D1-4FEB-9876-BB3C3C40EE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A41CD40D-2004-4BE0-AC6D-DC11522F2A1C}"/>
   <bookViews>
-    <workbookView xWindow="792" yWindow="720" windowWidth="22944" windowHeight="12336" activeTab="2" xr2:uid="{713376E4-D4C3-4AD6-8C36-1D956A9FD668}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{713376E4-D4C3-4AD6-8C36-1D956A9FD668}"/>
   </bookViews>
   <sheets>
     <sheet name="moefrags" sheetId="28" r:id="rId1"/>
@@ -685,28 +685,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{417C3CA6-4ECB-4F9B-A1AB-C587BD86D6A6}">
   <dimension ref="A1:BR59"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:M22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.6640625" style="2" customWidth="1"/>
-    <col min="8" max="13" width="8.88671875" style="2"/>
+    <col min="1" max="2" width="8.90625" style="2"/>
+    <col min="3" max="5" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.6328125" style="2" customWidth="1"/>
+    <col min="8" max="13" width="8.90625" style="2"/>
     <col min="14" max="19" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="21" max="22" width="8.88671875" style="2" customWidth="1"/>
-    <col min="23" max="36" width="8.88671875" style="2"/>
-    <col min="37" max="37" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="43" width="8.88671875" style="2"/>
-    <col min="44" max="46" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="49" width="9.33203125" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="8.88671875" style="2"/>
+    <col min="20" max="20" width="8.90625" style="2" hidden="1" customWidth="1"/>
+    <col min="21" max="22" width="8.90625" style="2" customWidth="1"/>
+    <col min="23" max="36" width="8.90625" style="2"/>
+    <col min="37" max="37" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="43" width="8.90625" style="2"/>
+    <col min="44" max="46" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="9.36328125" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.35">
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
@@ -878,7 +878,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>44</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>45</v>
       </c>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="AI7" s="6"/>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="AI8" s="6"/>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="AI9" s="6"/>
     </row>
-    <row r="10" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>46</v>
       </c>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="AW11" s="11"/>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>26</v>
@@ -2357,7 +2357,7 @@
       </c>
       <c r="AW12" s="11"/>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="AW13" s="11"/>
     </row>
-    <row r="14" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="AW14" s="18"/>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>48</v>
       </c>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="AI15" s="6"/>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="AI16" s="6"/>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="AI17" s="6"/>
     </row>
-    <row r="18" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="AI18" s="7"/>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
@@ -3164,7 +3164,7 @@
       </c>
       <c r="AS19" s="11"/>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>28</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -3619,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -3693,7 +3693,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O26" s="7">
         <f t="shared" si="24"/>
         <v>0</v>
@@ -3781,7 +3781,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -3930,7 +3930,7 @@
         <v>8.7401260870648631E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -4078,7 +4078,7 @@
         <v>6.3008887233249961E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -4226,7 +4226,7 @@
         <v>0.29969739292364994</v>
       </c>
     </row>
-    <row r="30" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O30" s="7">
         <f t="shared" si="24"/>
         <v>0</v>
@@ -4364,7 +4364,7 @@
         <v>0.1138657305835893</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -4489,7 +4489,7 @@
         <v>4.4523540296052627E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -4557,7 +4557,7 @@
       <c r="AZ32" s="11"/>
       <c r="BB32" s="11"/>
     </row>
-    <row r="33" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:69" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -4646,7 +4646,7 @@
       <c r="AZ33" s="11"/>
       <c r="BB33" s="11"/>
     </row>
-    <row r="34" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O34" s="7">
         <f t="shared" si="24"/>
         <v>0</v>
@@ -4725,7 +4725,7 @@
       <c r="AZ34" s="11"/>
       <c r="BB34" s="18"/>
     </row>
-    <row r="35" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AQ35" s="24" t="s">
         <v>27</v>
       </c>
@@ -4751,7 +4751,7 @@
       </c>
       <c r="AW35" s="10"/>
     </row>
-    <row r="36" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AQ36" s="24" t="s">
         <v>28</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -4858,13 +4858,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX39" s="3" t="s">
         <v>36</v>
       </c>
       <c r="AY39" s="3"/>
     </row>
-    <row r="40" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX40" s="2" t="s">
         <v>44</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>dE</v>
       </c>
     </row>
-    <row r="41" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX41" s="2" t="s">
         <v>45</v>
       </c>
@@ -4882,7 +4882,7 @@
         <v>dE(class)</v>
       </c>
     </row>
-    <row r="42" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX42" s="2" t="s">
         <v>46</v>
       </c>
@@ -4891,7 +4891,7 @@
         <v>dU</v>
       </c>
     </row>
-    <row r="43" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX43" s="3" t="s">
         <v>48</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>dU(class)</v>
       </c>
     </row>
-    <row r="44" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX44" s="2" t="s">
         <v>47</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>dE</v>
       </c>
     </row>
-    <row r="49" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="49" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX49" s="2" t="s">
         <v>37</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="50" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX50" s="2" t="s">
         <v>25</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="51" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX51" s="2" t="s">
         <v>26</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="52" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX52" s="2" t="s">
         <v>27</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="53" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX53" s="2" t="s">
         <v>28</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="55" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX55" s="2" t="s">
         <v>37</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="56" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX56" s="2" t="s">
         <v>25</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="57" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX57" s="2" t="s">
         <v>26</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="58" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX58" s="2" t="s">
         <v>27</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="59" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX59" s="2" t="s">
         <v>28</v>
       </c>
@@ -5026,28 +5026,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C9014C-F4F9-4570-85AB-3AE6AF329E11}">
   <dimension ref="A1:BR59"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:M22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.6640625" style="2" customWidth="1"/>
-    <col min="8" max="13" width="8.88671875" style="2"/>
+    <col min="1" max="2" width="8.90625" style="2"/>
+    <col min="3" max="5" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.6328125" style="2" customWidth="1"/>
+    <col min="8" max="13" width="8.90625" style="2"/>
     <col min="14" max="19" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="20" max="21" width="8.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="8.88671875" style="2" customWidth="1"/>
-    <col min="23" max="36" width="8.88671875" style="2"/>
-    <col min="37" max="37" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="43" width="8.88671875" style="2"/>
-    <col min="44" max="46" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="49" width="9.33203125" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="8.88671875" style="2"/>
+    <col min="20" max="21" width="8.90625" style="2" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="8.90625" style="2" customWidth="1"/>
+    <col min="23" max="36" width="8.90625" style="2"/>
+    <col min="37" max="37" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="43" width="8.90625" style="2"/>
+    <col min="44" max="46" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="9.36328125" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.35">
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>44</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -5804,7 +5804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>45</v>
       </c>
@@ -6108,7 +6108,7 @@
       </c>
       <c r="AI7" s="6"/>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
@@ -6215,7 +6215,7 @@
       </c>
       <c r="AI8" s="6"/>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -6322,7 +6322,7 @@
       </c>
       <c r="AI9" s="6"/>
     </row>
-    <row r="10" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>46</v>
       </c>
@@ -6566,7 +6566,7 @@
       </c>
       <c r="AW11" s="11"/>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>26</v>
@@ -6698,7 +6698,7 @@
       </c>
       <c r="AW12" s="11"/>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
@@ -6829,7 +6829,7 @@
       </c>
       <c r="AW13" s="11"/>
     </row>
-    <row r="14" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -6960,7 +6960,7 @@
       </c>
       <c r="AW14" s="18"/>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>48</v>
       </c>
@@ -7070,7 +7070,7 @@
       </c>
       <c r="AI15" s="6"/>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
@@ -7177,7 +7177,7 @@
       </c>
       <c r="AI16" s="6"/>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -7284,7 +7284,7 @@
       </c>
       <c r="AI17" s="6"/>
     </row>
-    <row r="18" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
@@ -7391,7 +7391,7 @@
       </c>
       <c r="AI18" s="7"/>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
@@ -7505,7 +7505,7 @@
       </c>
       <c r="AS19" s="11"/>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
@@ -7725,7 +7725,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>28</v>
       </c>
@@ -7835,7 +7835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -7898,7 +7898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -7960,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -8034,7 +8034,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O26" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -8122,7 +8122,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -8271,7 +8271,7 @@
         <v>0.25283882783882783</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -8419,7 +8419,7 @@
         <v>7.4203999092053413E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -8567,7 +8567,7 @@
         <v>0.25830863071485577</v>
       </c>
     </row>
-    <row r="30" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O30" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -8705,7 +8705,7 @@
         <v>0.75943396226415094</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -8830,7 +8830,7 @@
         <v>4.2317708333333329E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -8898,7 +8898,7 @@
       <c r="AZ32" s="11"/>
       <c r="BB32" s="11"/>
     </row>
-    <row r="33" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:69" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -8987,7 +8987,7 @@
       <c r="AZ33" s="11"/>
       <c r="BB33" s="11"/>
     </row>
-    <row r="34" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O34" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -9066,7 +9066,7 @@
       <c r="AZ34" s="11"/>
       <c r="BB34" s="18"/>
     </row>
-    <row r="35" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AQ35" s="24" t="s">
         <v>27</v>
       </c>
@@ -9092,7 +9092,7 @@
       </c>
       <c r="AW35" s="10"/>
     </row>
-    <row r="36" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AQ36" s="24" t="s">
         <v>28</v>
       </c>
@@ -9153,7 +9153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -9199,13 +9199,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX39" s="3" t="s">
         <v>36</v>
       </c>
       <c r="AY39" s="3"/>
     </row>
-    <row r="40" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX40" s="2" t="s">
         <v>44</v>
       </c>
@@ -9214,7 +9214,7 @@
         <v>dU</v>
       </c>
     </row>
-    <row r="41" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX41" s="2" t="s">
         <v>45</v>
       </c>
@@ -9223,7 +9223,7 @@
         <v>dU(class)</v>
       </c>
     </row>
-    <row r="42" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX42" s="2" t="s">
         <v>46</v>
       </c>
@@ -9232,7 +9232,7 @@
         <v>dU</v>
       </c>
     </row>
-    <row r="43" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX43" s="3" t="s">
         <v>48</v>
       </c>
@@ -9241,7 +9241,7 @@
         <v>dU</v>
       </c>
     </row>
-    <row r="44" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX44" s="2" t="s">
         <v>47</v>
       </c>
@@ -9250,7 +9250,7 @@
         <v>dE</v>
       </c>
     </row>
-    <row r="49" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="49" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX49" s="2" t="s">
         <v>37</v>
       </c>
@@ -9258,7 +9258,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="50" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX50" s="2" t="s">
         <v>25</v>
       </c>
@@ -9267,7 +9267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="51" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX51" s="2" t="s">
         <v>26</v>
       </c>
@@ -9276,7 +9276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="52" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX52" s="2" t="s">
         <v>27</v>
       </c>
@@ -9285,7 +9285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="53" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX53" s="2" t="s">
         <v>28</v>
       </c>
@@ -9294,7 +9294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="55" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX55" s="2" t="s">
         <v>37</v>
       </c>
@@ -9305,7 +9305,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="56" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX56" s="2" t="s">
         <v>25</v>
       </c>
@@ -9318,7 +9318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="57" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX57" s="2" t="s">
         <v>26</v>
       </c>
@@ -9331,7 +9331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="58" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX58" s="2" t="s">
         <v>27</v>
       </c>
@@ -9344,7 +9344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="59" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX59" s="2" t="s">
         <v>28</v>
       </c>
@@ -9367,28 +9367,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267B5DB3-6000-4DE5-B05F-26852CAE2384}">
   <dimension ref="A1:BR59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:M22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.6640625" style="2" customWidth="1"/>
-    <col min="8" max="13" width="8.88671875" style="2"/>
+    <col min="1" max="2" width="8.90625" style="2"/>
+    <col min="3" max="5" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.6328125" style="2" customWidth="1"/>
+    <col min="8" max="13" width="8.90625" style="2"/>
     <col min="14" max="19" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="21" max="22" width="8.88671875" style="2" customWidth="1"/>
-    <col min="23" max="36" width="8.88671875" style="2"/>
-    <col min="37" max="37" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="43" width="8.88671875" style="2"/>
-    <col min="44" max="46" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="49" width="9.33203125" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="8.88671875" style="2"/>
+    <col min="20" max="20" width="8.90625" style="2" hidden="1" customWidth="1"/>
+    <col min="21" max="22" width="8.90625" style="2" customWidth="1"/>
+    <col min="23" max="36" width="8.90625" style="2"/>
+    <col min="37" max="37" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="43" width="8.90625" style="2"/>
+    <col min="44" max="46" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="9.36328125" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.35">
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9420,7 +9420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
@@ -9560,7 +9560,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>44</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
@@ -9951,7 +9951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -10145,7 +10145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -10339,7 +10339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>45</v>
       </c>
@@ -10449,7 +10449,7 @@
       </c>
       <c r="AI7" s="6"/>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
@@ -10556,7 +10556,7 @@
       </c>
       <c r="AI8" s="6"/>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -10663,7 +10663,7 @@
       </c>
       <c r="AI9" s="6"/>
     </row>
-    <row r="10" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
@@ -10773,7 +10773,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>46</v>
       </c>
@@ -10907,7 +10907,7 @@
       </c>
       <c r="AW11" s="11"/>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>26</v>
@@ -11039,7 +11039,7 @@
       </c>
       <c r="AW12" s="11"/>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
@@ -11170,7 +11170,7 @@
       </c>
       <c r="AW13" s="11"/>
     </row>
-    <row r="14" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -11301,7 +11301,7 @@
       </c>
       <c r="AW14" s="18"/>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>48</v>
       </c>
@@ -11411,7 +11411,7 @@
       </c>
       <c r="AI15" s="6"/>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
@@ -11518,7 +11518,7 @@
       </c>
       <c r="AI16" s="6"/>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -11625,7 +11625,7 @@
       </c>
       <c r="AI17" s="6"/>
     </row>
-    <row r="18" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
@@ -11732,7 +11732,7 @@
       </c>
       <c r="AI18" s="7"/>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
@@ -11846,7 +11846,7 @@
       </c>
       <c r="AS19" s="11"/>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
@@ -11956,7 +11956,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
@@ -12066,7 +12066,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>28</v>
       </c>
@@ -12176,7 +12176,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -12239,7 +12239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -12301,7 +12301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -12375,7 +12375,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O26" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -12463,7 +12463,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -12612,7 +12612,7 @@
         <v>0.37809447496947496</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -12760,7 +12760,7 @@
         <v>3.9690163224035832E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -12908,7 +12908,7 @@
         <v>0.12713962938223625</v>
       </c>
     </row>
-    <row r="30" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O30" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -13046,7 +13046,7 @@
         <v>0.10269284750279706</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -13171,7 +13171,7 @@
         <v>4.2837685032894736E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -13239,7 +13239,7 @@
       <c r="AZ32" s="11"/>
       <c r="BB32" s="11"/>
     </row>
-    <row r="33" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:69" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -13328,7 +13328,7 @@
       <c r="AZ33" s="11"/>
       <c r="BB33" s="11"/>
     </row>
-    <row r="34" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O34" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -13407,7 +13407,7 @@
       <c r="AZ34" s="11"/>
       <c r="BB34" s="18"/>
     </row>
-    <row r="35" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AQ35" s="24" t="s">
         <v>27</v>
       </c>
@@ -13433,7 +13433,7 @@
       </c>
       <c r="AW35" s="10"/>
     </row>
-    <row r="36" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AQ36" s="24" t="s">
         <v>28</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -13540,13 +13540,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX39" s="3" t="s">
         <v>36</v>
       </c>
       <c r="AY39" s="3"/>
     </row>
-    <row r="40" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX40" s="2" t="s">
         <v>44</v>
       </c>
@@ -13555,7 +13555,7 @@
         <v>dU</v>
       </c>
     </row>
-    <row r="41" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX41" s="2" t="s">
         <v>45</v>
       </c>
@@ -13564,7 +13564,7 @@
         <v>dE</v>
       </c>
     </row>
-    <row r="42" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX42" s="2" t="s">
         <v>46</v>
       </c>
@@ -13573,7 +13573,7 @@
         <v>dE</v>
       </c>
     </row>
-    <row r="43" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX43" s="3" t="s">
         <v>48</v>
       </c>
@@ -13582,7 +13582,7 @@
         <v>dE(class)</v>
       </c>
     </row>
-    <row r="44" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX44" s="2" t="s">
         <v>47</v>
       </c>
@@ -13591,7 +13591,7 @@
         <v>dE</v>
       </c>
     </row>
-    <row r="49" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="49" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX49" s="2" t="s">
         <v>37</v>
       </c>
@@ -13599,7 +13599,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="50" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX50" s="2" t="s">
         <v>25</v>
       </c>
@@ -13608,7 +13608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="51" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX51" s="2" t="s">
         <v>26</v>
       </c>
@@ -13617,7 +13617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="52" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX52" s="2" t="s">
         <v>27</v>
       </c>
@@ -13626,7 +13626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="53" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX53" s="2" t="s">
         <v>28</v>
       </c>
@@ -13635,7 +13635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="55" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX55" s="2" t="s">
         <v>37</v>
       </c>
@@ -13646,7 +13646,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="56" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX56" s="2" t="s">
         <v>25</v>
       </c>
@@ -13659,7 +13659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="57" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX57" s="2" t="s">
         <v>26</v>
       </c>
@@ -13672,7 +13672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="58" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX58" s="2" t="s">
         <v>27</v>
       </c>
@@ -13685,7 +13685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="59" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX59" s="2" t="s">
         <v>28</v>
       </c>
@@ -13709,27 +13709,27 @@
   <dimension ref="A1:BR59"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:M18"/>
+      <selection activeCell="C15" sqref="C15:M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.6640625" style="2" customWidth="1"/>
-    <col min="8" max="13" width="8.88671875" style="2"/>
+    <col min="1" max="2" width="8.90625" style="2"/>
+    <col min="3" max="5" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.6328125" style="2" customWidth="1"/>
+    <col min="8" max="13" width="8.90625" style="2"/>
     <col min="14" max="19" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="21" max="22" width="8.88671875" style="2" customWidth="1"/>
-    <col min="23" max="36" width="8.88671875" style="2"/>
-    <col min="37" max="37" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="43" width="8.88671875" style="2"/>
-    <col min="44" max="46" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="49" width="9.33203125" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="8.88671875" style="2"/>
+    <col min="20" max="20" width="8.90625" style="2" hidden="1" customWidth="1"/>
+    <col min="21" max="22" width="8.90625" style="2" customWidth="1"/>
+    <col min="23" max="36" width="8.90625" style="2"/>
+    <col min="37" max="37" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="43" width="8.90625" style="2"/>
+    <col min="44" max="46" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="9.36328125" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.35">
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
@@ -13761,7 +13761,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
@@ -13901,7 +13901,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>44</v>
       </c>
@@ -14098,7 +14098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
@@ -14292,7 +14292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -14486,7 +14486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -14680,7 +14680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>45</v>
       </c>
@@ -14790,7 +14790,7 @@
       </c>
       <c r="AI7" s="6"/>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
@@ -14897,7 +14897,7 @@
       </c>
       <c r="AI8" s="6"/>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -15004,7 +15004,7 @@
       </c>
       <c r="AI9" s="6"/>
     </row>
-    <row r="10" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
@@ -15114,7 +15114,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>46</v>
       </c>
@@ -15248,7 +15248,7 @@
       </c>
       <c r="AW11" s="11"/>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>26</v>
@@ -15380,7 +15380,7 @@
       </c>
       <c r="AW12" s="11"/>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
@@ -15511,7 +15511,7 @@
       </c>
       <c r="AW13" s="11"/>
     </row>
-    <row r="14" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -15642,7 +15642,7 @@
       </c>
       <c r="AW14" s="18"/>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>48</v>
       </c>
@@ -15752,7 +15752,7 @@
       </c>
       <c r="AI15" s="6"/>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
@@ -15859,7 +15859,7 @@
       </c>
       <c r="AI16" s="6"/>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -15966,7 +15966,7 @@
       </c>
       <c r="AI17" s="6"/>
     </row>
-    <row r="18" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
@@ -16073,7 +16073,7 @@
       </c>
       <c r="AI18" s="7"/>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
@@ -16187,7 +16187,7 @@
       </c>
       <c r="AS19" s="11"/>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
@@ -16297,7 +16297,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
@@ -16407,7 +16407,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>28</v>
       </c>
@@ -16517,7 +16517,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -16580,7 +16580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -16642,7 +16642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -16716,7 +16716,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O26" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -16804,7 +16804,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -16953,7 +16953,7 @@
         <v>0.25283882783882783</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -17101,7 +17101,7 @@
         <v>8.1778004161059889E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -17249,7 +17249,7 @@
         <v>0.13683976637887252</v>
       </c>
     </row>
-    <row r="30" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O30" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -17387,7 +17387,7 @@
         <v>0.19464403247038173</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -17512,7 +17512,7 @@
         <v>5.1740241928703551E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -17580,7 +17580,7 @@
       <c r="AZ32" s="11"/>
       <c r="BB32" s="11"/>
     </row>
-    <row r="33" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:69" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -17669,7 +17669,7 @@
       <c r="AZ33" s="11"/>
       <c r="BB33" s="11"/>
     </row>
-    <row r="34" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O34" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -17748,7 +17748,7 @@
       <c r="AZ34" s="11"/>
       <c r="BB34" s="18"/>
     </row>
-    <row r="35" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AQ35" s="24" t="s">
         <v>27</v>
       </c>
@@ -17774,7 +17774,7 @@
       </c>
       <c r="AW35" s="10"/>
     </row>
-    <row r="36" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AQ36" s="24" t="s">
         <v>28</v>
       </c>
@@ -17835,7 +17835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -17881,7 +17881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX39" s="3" t="s">
         <v>36</v>
       </c>
@@ -17890,7 +17890,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX40" s="2" t="s">
         <v>44</v>
       </c>
@@ -17903,7 +17903,7 @@
         <v>2.92 (0.25)</v>
       </c>
     </row>
-    <row r="41" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX41" s="2" t="s">
         <v>45</v>
       </c>
@@ -17916,7 +17916,7 @@
         <v>1.01 (0.12)</v>
       </c>
     </row>
-    <row r="42" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX42" s="2" t="s">
         <v>46</v>
       </c>
@@ -17929,7 +17929,7 @@
         <v>2.6 (0.18)</v>
       </c>
     </row>
-    <row r="43" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX43" s="3" t="s">
         <v>48</v>
       </c>
@@ -17942,7 +17942,7 @@
         <v>10.74 (0.75)</v>
       </c>
     </row>
-    <row r="44" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX44" s="2" t="s">
         <v>47</v>
       </c>
@@ -17955,7 +17955,7 @@
         <v>1.43 (0.11)</v>
       </c>
     </row>
-    <row r="49" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="49" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX49" s="2" t="s">
         <v>37</v>
       </c>
@@ -17963,7 +17963,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="50" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX50" s="2" t="s">
         <v>25</v>
       </c>
@@ -17972,7 +17972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="51" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX51" s="2" t="s">
         <v>26</v>
       </c>
@@ -17981,7 +17981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="52" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX52" s="2" t="s">
         <v>27</v>
       </c>
@@ -17990,7 +17990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="53" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX53" s="2" t="s">
         <v>28</v>
       </c>
@@ -17999,7 +17999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="55" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX55" s="2" t="s">
         <v>37</v>
       </c>
@@ -18010,7 +18010,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="56" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX56" s="2" t="s">
         <v>25</v>
       </c>
@@ -18023,7 +18023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="57" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX57" s="2" t="s">
         <v>26</v>
       </c>
@@ -18036,7 +18036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="58" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX58" s="2" t="s">
         <v>27</v>
       </c>
@@ -18049,7 +18049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="59" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX59" s="2" t="s">
         <v>28</v>
       </c>
@@ -18072,28 +18072,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A1308B0-E661-4D8B-BA70-0F60D2750615}">
   <dimension ref="A1:BR59"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:M18"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AZ27" sqref="AZ27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.6640625" style="2" customWidth="1"/>
-    <col min="8" max="13" width="8.88671875" style="2"/>
+    <col min="1" max="2" width="8.90625" style="2"/>
+    <col min="3" max="5" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.6328125" style="2" customWidth="1"/>
+    <col min="8" max="13" width="8.90625" style="2"/>
     <col min="14" max="19" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="2" hidden="1" customWidth="1"/>
-    <col min="21" max="22" width="8.88671875" style="2" customWidth="1"/>
-    <col min="23" max="36" width="8.88671875" style="2"/>
-    <col min="37" max="37" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="43" width="8.88671875" style="2"/>
-    <col min="44" max="46" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="49" width="9.33203125" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="8.88671875" style="2"/>
+    <col min="20" max="20" width="8.90625" style="2" hidden="1" customWidth="1"/>
+    <col min="21" max="22" width="8.90625" style="2" customWidth="1"/>
+    <col min="23" max="36" width="8.90625" style="2"/>
+    <col min="37" max="37" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="43" width="8.90625" style="2"/>
+    <col min="44" max="46" width="9.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="9.36328125" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.35">
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
@@ -18125,7 +18125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
@@ -18265,7 +18265,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>44</v>
       </c>
@@ -18462,7 +18462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
@@ -18656,7 +18656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
@@ -18850,7 +18850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
@@ -19044,7 +19044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>45</v>
       </c>
@@ -19154,7 +19154,7 @@
       </c>
       <c r="AI7" s="6"/>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
@@ -19261,7 +19261,7 @@
       </c>
       <c r="AI8" s="6"/>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
@@ -19368,7 +19368,7 @@
       </c>
       <c r="AI9" s="6"/>
     </row>
-    <row r="10" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
@@ -19478,7 +19478,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>46</v>
       </c>
@@ -19612,7 +19612,7 @@
       </c>
       <c r="AW11" s="11"/>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>26</v>
@@ -19744,7 +19744,7 @@
       </c>
       <c r="AW12" s="11"/>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
@@ -19875,7 +19875,7 @@
       </c>
       <c r="AW13" s="11"/>
     </row>
-    <row r="14" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:60" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -20006,7 +20006,7 @@
       </c>
       <c r="AW14" s="18"/>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>48</v>
       </c>
@@ -20116,7 +20116,7 @@
       </c>
       <c r="AI15" s="6"/>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:60" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
@@ -20223,7 +20223,7 @@
       </c>
       <c r="AI16" s="6"/>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -20330,7 +20330,7 @@
       </c>
       <c r="AI17" s="6"/>
     </row>
-    <row r="18" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>28</v>
       </c>
@@ -20437,7 +20437,7 @@
       </c>
       <c r="AI18" s="7"/>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>47</v>
       </c>
@@ -20551,7 +20551,7 @@
       </c>
       <c r="AS19" s="11"/>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
@@ -20661,7 +20661,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
@@ -20771,7 +20771,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>28</v>
       </c>
@@ -20881,7 +20881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -20944,7 +20944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -21006,7 +21006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -21080,7 +21080,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O26" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -21168,7 +21168,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -21317,7 +21317,7 @@
         <v>0.37809447496947496</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -21465,7 +21465,7 @@
         <v>3.9690163224035832E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -21613,7 +21613,7 @@
         <v>0.12713962938223625</v>
       </c>
     </row>
-    <row r="30" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:70" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O30" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -21751,7 +21751,7 @@
         <v>0.10269284750279706</v>
       </c>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -21876,7 +21876,7 @@
         <v>4.2837685032894736E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -21944,7 +21944,7 @@
       <c r="AZ32" s="11"/>
       <c r="BB32" s="11"/>
     </row>
-    <row r="33" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:69" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -22033,7 +22033,7 @@
       <c r="AZ33" s="11"/>
       <c r="BB33" s="11"/>
     </row>
-    <row r="34" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="O34" s="7">
         <f t="shared" si="23"/>
         <v>0</v>
@@ -22112,7 +22112,7 @@
       <c r="AZ34" s="11"/>
       <c r="BB34" s="18"/>
     </row>
-    <row r="35" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AQ35" s="24" t="s">
         <v>27</v>
       </c>
@@ -22138,7 +22138,7 @@
       </c>
       <c r="AW35" s="10"/>
     </row>
-    <row r="36" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AQ36" s="24" t="s">
         <v>28</v>
       </c>
@@ -22199,7 +22199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -22245,7 +22245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX39" s="3" t="s">
         <v>36</v>
       </c>
@@ -22254,7 +22254,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX40" s="2" t="s">
         <v>44</v>
       </c>
@@ -22267,7 +22267,7 @@
         <v>4.38 (0.38)</v>
       </c>
     </row>
-    <row r="41" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX41" s="2" t="s">
         <v>45</v>
       </c>
@@ -22280,7 +22280,7 @@
         <v>1.47 (0.18)</v>
       </c>
     </row>
-    <row r="42" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX42" s="2" t="s">
         <v>46</v>
       </c>
@@ -22293,7 +22293,7 @@
         <v>2.63 (0.14)</v>
       </c>
     </row>
-    <row r="43" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX43" s="3" t="s">
         <v>48</v>
       </c>
@@ -22306,7 +22306,7 @@
         <v>10.74 (0.75)</v>
       </c>
     </row>
-    <row r="44" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:69" x14ac:dyDescent="0.35">
       <c r="AX44" s="2" t="s">
         <v>47</v>
       </c>
@@ -22319,7 +22319,7 @@
         <v>2.1 (0.17)</v>
       </c>
     </row>
-    <row r="49" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="49" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX49" s="2" t="s">
         <v>37</v>
       </c>
@@ -22327,7 +22327,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="50" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX50" s="2" t="s">
         <v>25</v>
       </c>
@@ -22336,7 +22336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="51" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX51" s="2" t="s">
         <v>26</v>
       </c>
@@ -22345,7 +22345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="52" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX52" s="2" t="s">
         <v>27</v>
       </c>
@@ -22354,7 +22354,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="53" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX53" s="2" t="s">
         <v>28</v>
       </c>
@@ -22363,7 +22363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="55" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX55" s="2" t="s">
         <v>37</v>
       </c>
@@ -22374,7 +22374,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="56" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX56" s="2" t="s">
         <v>25</v>
       </c>
@@ -22387,7 +22387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="57" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX57" s="2" t="s">
         <v>26</v>
       </c>
@@ -22400,7 +22400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="58" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX58" s="2" t="s">
         <v>27</v>
       </c>
@@ -22413,7 +22413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="50:52" x14ac:dyDescent="0.3">
+    <row r="59" spans="50:52" x14ac:dyDescent="0.35">
       <c r="AX59" s="2" t="s">
         <v>28</v>
       </c>
@@ -22442,12 +22442,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100716B8B8961709E49859A44A6608C242D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="91f316d38f2be5494ab0d3724e124308">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="43b54cb5-a873-4f5e-a135-b4610bf181d2" xmlns:ns4="d028fd66-6788-42b6-b8bb-de8ad7a52eae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="96c47c95b784b6b02f3b818bccb484f5" ns3:_="" ns4:_="">
     <xsd:import namespace="43b54cb5-a873-4f5e-a135-b4610bf181d2"/>
@@ -22664,6 +22658,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53CBEE6-5899-4AD1-8B90-40A1FC5D2C26}">
   <ds:schemaRefs>
@@ -22673,23 +22673,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F74EE212-7898-4CD6-8DA3-5A159F1B056F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="43b54cb5-a873-4f5e-a135-b4610bf181d2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d028fd66-6788-42b6-b8bb-de8ad7a52eae"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F103E5DF-3271-444E-82FA-6EB6E6C41388}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22706,4 +22689,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F74EE212-7898-4CD6-8DA3-5A159F1B056F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="43b54cb5-a873-4f5e-a135-b4610bf181d2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d028fd66-6788-42b6-b8bb-de8ad7a52eae"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>